<commit_message>
Initial Streamlit UI / Gemini Integration / Confidence Answering
</commit_message>
<xml_diff>
--- a/data/ground_truth.xlsx
+++ b/data/ground_truth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chana\OneDrive\Desktop\MLStudy\LangChain\langchain_learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chana\OneDrive\Desktop\MLStudy\LangChain\Document_Searcher_RAG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE37997-F091-4C1C-91C9-273D5821EF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED29568-7271-4C36-A010-C6A936C9DF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{545F1D67-D6F6-418E-A279-856261A0F0C2}"/>
   </bookViews>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H137" sqref="H137"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>